<commit_message>
update data for near & modified copy
</commit_message>
<xml_diff>
--- a/test_data/near_modified_copy.xlsx
+++ b/test_data/near_modified_copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rosen\Desktop\vietnamese_plagiarism\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABB17F2-77FB-4A22-BDB3-8638D1B263B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F50E294-E8DD-4D58-818C-896513EEB908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{1B652FA6-7F9E-457D-896F-C49F6D08CB98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="115">
   <si>
     <t>no.</t>
   </si>
@@ -314,6 +314,119 @@
   <si>
     <t>Hầu hết các thông tin trong chính phủ, công nghiệp, thương mại và các viện nghiên cứu đều được lưu trữ ở dạng điện tử, theo kiểu cơ sở dữ liệu văn bản. Số lượng tài liệu điện tử này phát triển với tốc độ chóng mặt gây cho con người những khó khăn trong việc tiếp nhận nội dung chính của chúng.
 Các kỹ thuật tìm kiếm thông tin truyền thống trở nên không tương xứng với lượng dữ liệu văn bản ngày càng lớn. Người dùng không biết bên trong tài liệu chứa gì, thật khó để đưa ra câu truy vấn hiệu quả cho việc phân tích và trích rút các thông tin có ích từ dữ liệu. Người sử dụng cần các công cụ so sánh các tài liệu khác nhau, xếp hạng độ quan trọng và độ liên quan của các tài liệu, hoặc tìm các mẫu và các xu hướng qua nhiều tài liệu. Do đó, việc tính độ tương đồng trong văn bản, độ tương đồng giữa các văn bản, tóm tắt văn bản ... trở nên ngày càng phổ biến và là nội dung cần thiết trong khai phá text</t>
+  </si>
+  <si>
+    <t>Cạnh tranh giữa các công ty ngày càng gay gắt. Theo Sharma, Agarwal, Dhir và Sikka (2016), không thể có được khách hàng nếu không biết nhu cầu của họ. Một cách để tìm hiểu xem khách hàng có phù hợp với bạn hay không là để họ dùng thử sản phẩm của bạn. Tiếp theo, đánh giá mức độ hài lòng của khách hàng đối với sản phẩm hoặc dịch vụ. Nhưng câu hỏi đặt ra là, làm thế nào một công ty có thể biết được khách hàng của mình hài lòng hay không hài lòng về vấn đề này, hoặc thương hiệu của họ có được người dùng sử dụng thường xuyên hay không? Để giải quyết vấn đề này, nghiên cứu đề xuất giải pháp tận dụng ý kiến ​​của khách hàng về sản phẩm của  cửa hàng để lại trên trang web Foody. Tuy nhiên, dữ liệu  ở mức độ thô sơ  và lượng dữ liệu quá lớn nên các công ty không thể đưa ra quyết định dựa trên dữ liệu thô này và cần phải biết những kiến ​​thức được phân tích từ tập dữ liệu này mà mình có được. Do đó, chúng tôi đã áp dụng kỹ thuật học máy để phân loại dữ liệu, xem nhận xét nào  tích  cực và tiêu cực, đồng thời sử dụng các kỹ thuật phân tích và dự đoán. Cuối cùng, chúng tôi khám phá các công cụ khai thác  để trực quan hóa dữ liệu trong các báo cáo thông minh (trang tổng quan). Các phát hiện giúp các công ty và lãnh đạo doanh nghiệp có được thông tin  dễ dàng và nhanh chóng, từ đó  cải thiện và nâng cao sự phát triển kinh doanh.</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>Trong hai thập kỷ qua, các phương pháp dựa trên máy học  đã thống trị  hầu hết các bài toán phân tích cảm tính, đặc biệt là các bài toán cấp độ văn bản. Điều này là do việc trình bày đặc điểm có tác động đáng kể đến hiệu suất của phân tích cảm tính. Nghiên cứu đã tập trung vào việc tạo ra các bộ tính năng hiệu quả dựa trên kiến ​​thức miền và các kỹ thuật chuyên ngành điển hình như các công trình [10], [11]. Khi làm như vậy, các tác giả đã sử dụng ba kỹ thuật học máy truyền thống: Máy vectơ hỗ trợ (SVM), Naive Bayes (NB), và Entropy tối đa (ME) để tìm hiểu một tập dữ liệu có thuộc tính n-gram và thu được các kết quả thực nghiệm tương tự. thu được ngay cả với số nhị phân cao. hoặc phân loại nhiều cấp 
+ bằng cấp. Tuy nhiên, nhiệm vụ này  có thể được thực hiện tốt bằng cách học biểu diễn hoặc các thuật toán học tính năng như cách tiếp cận  học sâu, kỹ thuật nhận dạng tự động  và giải thích các biểu diễn dạng văn bản từ dữ liệu. Học sâu được sinh ra vì nó có thể tạo ra các biểu diễn dữ liệu ở nhiều cấp độ. Trong số đó có công trình của D. Nguyen và cộng sự [12], trong đó tài liệu  tiếng Việt được dịch bằng máy sang tài liệu tiếng Anh và sau đó trích xuất tính năng, khi sử dụng tài liệu tiếng Anh đã dịch làm dữ liệu đào tạo. Trong công việc này, CNN (Mạng lưới thần kinh chuyển đổi) được sử dụng để phân loại văn bản. Kết quả thử nghiệm đạt 84,40% trên tổng số 25.991 lượt đánh giá sản phẩm bằng tiếng Việt. [13] Tác giả Q. Vo et al. Sử dụng kết hợp hai mạng LSTM (Trí nhớ ngắn hạn dài) và CNN, 17.500 từ tiếng Việt theo ba mức khen, chê và trung lập khi phát hiện CNN thể hiện tốt trong phần bình luận của bộ sưu tập đã được xếp hạng. 
+ Các LSTM có bổ trợ trong văn bản và  cơ chế quên tôi không có thể xử lý  các  phụ thuộc từ xa trong văn bản.</t>
+  </si>
+  <si>
+    <t>Xử lý ngôn ngữ tự nhiên (NLP) là một nhánh của trí tuệ nhân tạo tập trung vào việc ứng dụng nó vào ngôn ngữ của con người. Xử lý ngôn ngữ tự nhiên là một trong những phần khó nhất của trí tuệ nhân tạo. Bởi vì nó là tất cả để hiểu ý nghĩa của ngôn ngữ, nó là công cụ hoàn hảo nhất để suy nghĩ và giao tiếp.  Xử lý giọng nói là xử lý thông tin khi đầu vào là "dữ liệu giọng nói" (dữ liệu được chuyển đổi), tức là dữ liệu "văn bản" hoặc "giọng nói". Dữ liệu liên quan đến ngôn ngữ viết (văn bản) và nói (giọng nói) đang ngày càng trở thành một loại dữ liệu thống trị. 
+ Sở hữu và lưu trữ dưới dạng điện tử. Đặc điểm chính của các kiểu dữ liệu này là chúng không có cấu trúc hoặc bán cấu trúc và  không thể được lưu trữ ở các định dạng cố định như bảng. Xử lý ngôn ngữ tự nhiên là một lĩnh vực nghiên cứu nhằm  cho phép các hệ thống máy tính hiểu và xử lý  ngôn ngữ của con người. Dịch máy là một trong những ứng dụng chính của xử lý ngôn ngữ tự nhiên.</t>
+  </si>
+  <si>
+    <t>Trong học máy, máy tính không thể hiểu  ngôn ngữ tự nhiên một cách trực tiếp, chỉ  khi nó được biểu diễn trong không gian vectơ. Các kích thước thuộc tính đầu vào  được biểu diễn dưới dạng ma trận vectơ. Có nhiều cách để biểu diễn văn bản trong ma trận vectơ, bao gồm các mô hình và phần mở rộng như các mô hình Word2Vec, GloVe và FastTex (Sarkar, 2019). Trong công việc này, chúng tôi áp dụng hai phương pháp, Bag of N-gram và TF-IDF, để kiểm tra mô hình và vẽ biểu đồ dữ liệu.</t>
+  </si>
+  <si>
+    <t>Theo đánh giá của  Oracle,  80% dữ liệu của con người hiện nay là dữ liệu phi cấu trúc  [Oracle Text]. Với sự lan rộng của Internet,  sách  điện tử,  máy tính cá nhân, thiết bị liên lạc, thiết bị âm thanh, v.v., giờ đây ai cũng có thể tạo  dữ liệu văn bản và giọng nói. Câu hỏi đặt ra là làm thế nào để chúng ta  xử lý chúng, tức là chuyển chúng từ  dạng khó hiểu  thành  dạng mà chúng ta có thể hiểu và diễn giải, tức là làm thế nào chúng ta có thể tìm thấy thông tin và kiến ​​thức hữu ích cho bản thân.</t>
+  </si>
+  <si>
+    <t>1. Nhận dạng giọng nói: Nhận dạng từ sóng giọng nói  và chuyển đổi sang dữ liệu văn bản tương ứng. Ví dụ, thay vì nhập tài liệu, người dùng đọc tài liệu  và trình soạn thảo viết tài liệu đó ra. Đây cũng là bước đầu tiên để hiện thực hóa giấc mơ  giao tiếp giữa  người và robot. Nhận dạng giọng nói rất hữu ích cho người khiếm thị. 
+2. Chuyển văn bản thành giọng nói: Phân tích dữ liệu văn bản và chuyển nó thành giọng nói của con người. Thay vì  đọc một cuốn sách hoặc trang web một mình, nó sẽ tự động đọc nó cho bạn. Giống như nhận dạng giọng nói, chuyển văn bản thành giọng nói là một công cụ tuyệt vời cho người khiếm thị, nhưng ngược lại, nó là giai đoạn cuối cùng của giao tiếp giữa người và robot. 
+ 3. Nhận dạng ký tự quang học (OCR): Nhận dạng từng ký tự từ văn bản in  và chuyển đổi thành  tệp văn bản trên máy tính của bạn. Có hai kiểu công nhận. Đầu tiên là nhận dạng văn bản in, chẳng hạn như văn bản sách giáo khoa và chuyển nó thành tài liệu điện tử, chẳng hạn như  định dạng doc của Microsoft Word. Viết tay, phức tạp hơn  nhận dạng chữ viết  tay và không có khuôn mẫu rõ ràng thay đổi theo từng người, là một thách thức, nhưng một chương trình nhận dạng chữ viết tay có thể biến hàng nghìn tiêu đề email thành tài liệu điện tử trong một khoảng thời gian ngắn. Nhận dạng chữ viết tay của con người có ứng dụng trong pháp y và bảo mật thông tin (nhận dạng chữ ký điện tử). 
+4. Dịch máy: Máy tính dịch  một tệp văn bản bằng một ngôn ngữ (chẳng hạn như tiếng Anh) sang một tệp văn bản bằng một ngôn ngữ khác. Phần mềm  tiếng Việt tiêu biểu cho chương trình này là Evtrans của Softex, phần mềm tự động dịch ứng dụng này từ tiếng Anh sang tiếng Việt và ngược lại trực tuyến. Có hai công ty làm việc trong lĩnh vực này của người Việt Nam. Lạc Việt (công ty xuất bản từ điển Lạc Việt) và Google.  
+5. Tóm tắt văn bản: Từ một văn bản dài (ví dụ 10 trang), máy sẽ tóm tắt  một văn bản ngắn (1 trang) chứa nội dung cơ bản.
+6. Tìm kiếm thông tin: Tìm các tệp tin  có nội dung liên quan đến  vấn đề (câu hỏi)  cần biết (hoặc câu trả lời) từ nhiều nguồn văn bản hoặc tệp âm thanh. Một ví dụ về công nghệ này là Google,  hệ thống truy xuất thông tin trên Internet mà hầu hết chúng ta sử dụng thường xuyên. Mặc dù  hiệu quả cao nhất, Google  có khả năng  tìm kiếm các câu hỏi dưới dạng  từ khóa, và vì nhiều tài liệu liên quan đã tồn tại, nó sẽ luôn "tìm kiếm" nhiều tài liệu không liên quan, ngược lại Google không thể tìm thấy nó. 
+7. Trích xuất thông tin: Từ nhiều nguồn  tệp văn bản hoặc âm thanh, tìm các đoạn của một vài tệp có liên quan đến các vấn đề đã biết hoặc các vấn đề (câu hỏi)  cần được giải đáp. Hệ thống trích xuất thông tin có thể được phân biệt với truy xuất thông tin bằng cách "truy cập" các trang web có liên quan, phân tích các trang và trích xuất thông tin mong muốn. 
+8. Khám phá kiến ​​thức và Khai thác dữ liệu văn bản: Có thể khám phá những kiến ​​thức chưa được khám phá trước đó từ nhiều nguồn tài liệu, ngay cả khi chúng có ít mối liên hệ với nhau. Đây là một vấn đề rất phức tạp và đang trong giai đoạn đầu  nghiên cứu trên khắp thế giới. có thể phân loại vấn đề 
+ - 1-3 trong lĩnh vực xử lý âm thanh và hình ảnh, 
+ - 4-5 trong lĩnh vực xử lý văn bản (xử lý văn bản), 
+ - 6-8 trong lĩnh vực Khai thác văn bản và web (Text and Web Mining).</t>
+  </si>
+  <si>
+    <t>Các hư từ cổ.
+Đây là danh mục bao gồm những từ hư không còn thiếu trong cuộc sống năng động của người Việt Nam hiện đại, đặc biệt hơn, đây là những  từ không còn được sử dụng trong giao tiếp thông thường hàng ngày. Danh sách những lời nguyền này bao gồm Phao (18 lần), Moore (35), Ring (32), Sa (23), Four (3), Fringe (11), Packet (18), Le (1), Roan (9) , Hòa (43), Tốt (20), Chung (45), Người bình (26), Giường (14), Ít (103), Khôn ngoan (53), Có thể (80), Lệ (1), Tình huống (10) , Xe tải (6), Hà (22), Hề (7), Nghiêm trọng (19), Dozen (7), Khá (21).</t>
+  </si>
+  <si>
+    <t>Tôi hy vọng rằng bài viết này một mặt có thể góp thêm một chút tiếng nói  vào việc nghiên cứu  vấn đề lớn về sự phù phiếm, mặt khác, những  giải thích trong bài báo sẽ giúp ích ít nhiều cho việc giảng dạy tiếng Việt cho người nước ngoài, chúng ta. một công việc được thực hiện bởi các bậc thầy đi trước  và được tiếp tục bởi chúng tôi và các thế hệ tương lai.</t>
+  </si>
+  <si>
+    <t>• Giới từ: Một lớp từ hư ảo được sử dụng để diễn đạt các mối quan hệ về không gian, thời gian, nguyên nhân, mục đích và các mối quan hệ khác giữa  các đối tượng và hoạt động, trạng thái hoặc phẩm chất. Trong cú pháp, giới từ được sử dụng để chỉ mối quan hệ cú pháp giữa  danh từ, tính từ, tính từ bắt nguồn  từ danh từ và số lượng từ, mối quan hệ giữa động từ và danh từ, đại từ và tính từ. Bản thân ý nghĩa  của giới từ không thể được thể hiện bên ngoài mối quan hệ của nó với một  dạng cụ thể.</t>
+  </si>
+  <si>
+    <t>Kỹ thuật làm sáng: Quá trình làm sáng hoặc làm sáng dữ liệu hình ảnh  cho phép mô hình có khả năng dự đoán tốt trong nhiều điều kiện ánh sáng  trong thế giới thực. Tuy nhiên, để tránh giảm ảnh quá tối hoặc quá sáng và khiến mô hình  học  dữ liệu xấu, việc tăng giảm độ sáng cũng cần được ghi lại ở các giá trị hợp lý.</t>
+  </si>
+  <si>
+    <t>Mục tiêu chính của Siamese là  tìm  cách ánh xạ  ảnh sang không gian vectơ n chiều để chúng ta không  phải  chọn hàm mất  entropy chéo nhị phân [18] như trong các bài toán phân loại nhị phân khác. Mô hình facenet là một chủ nghĩa hình thức của người Siemese có tác dụng  biểu diễn hình ảnh trong không gian vectơ n chiều sao cho khoảng cách giữa các vectơ nhúng càng nhỏ thì mức độ thành viên trong cùng một lớp của các ảnh tương ứng càng lớn.</t>
+  </si>
+  <si>
+    <t>Tại Việt Nam, việc ứng dụng  công nghệ nhận dạng khuôn mặt vào thực tế vẫn còn nhiều hạn chế. Mục tiêu của công việc này là tìm hiểu một số phương pháp nhận dạng khuôn mặt và áp dụng chúng vào thực tế để điều chỉnh chúng cho phù hợp với thực tế của đất nước.</t>
+  </si>
+  <si>
+    <t>Các đối tượng trực quan của EGM được hiển thị dưới dạng đồ thị có nhãn, với các nút đại diện cho các tính năng rời rạc dựa trên các wavelet Gabor  và các cạnh biểu thị khoảng cách giữa các vị trí nút trên  hình ảnh. Do đó, hình ảnh của một đối tượng được biểu diễn dưới dạng một tập hợp các đặc điểm đơn lẻ trong một cấu hình không gian cụ thể. Khi các đối tượng mới được phát hiện trong ảnh, một biểu đồ có nhãn của các đối tượng sẽ được lưu (gọi là biểu đồ  mô hình) và được liên kết với ảnh. Vị trí của  nút trong  hình ảnh cho mỗi biểu đồ mô hình 
+ Tối ưu hóa. Do đó, các đặc điểm nổi bật của hình ảnh được khớp trên các nút của mô hình. Đồ thị mô hình là lý tưởng cho các đối tượng được phát hiện và có thể tạo đồ thị hình ảnh dựa trên các vị trí nút  trong hình ảnh. Đối sánh đồ thị chùm đàn hồi (EBGM) là một phần mở rộng của EGM phù hợp với các lớp đặc trưng có  cấu trúc phổ phổ biến như: B. Một khuôn mặt trong cùng một tư thế. Tất cả các trường hợp có thể có của  lớp được biểu diễn bằng cùng một loại đồ thị. Đồ thị tạo ra các gói đồ thị có cùng  cấu trúc. Một nút đại diện cho kết cấu cục bộ của bất kỳ đối tượng nào trong  lớp  (ví dụ: tất cả các biến thể của mắt) và một  cạnh đại diện cho khoảng cách trung bình giữa các vị trí nút (ví dụ khoảng cách trung bình giữa các mao quản). Điều này cho phép  
+ Sử dụng kết hợp các tính năng khác nhau đại diện cho các trường hợp của các lớp tính năng ẩn. Ví dụ, bạn có thể lấy kết cấu mắt. 
+ Các họa tiết cho một khuôn mặt và  miệng cho khuôn mặt còn lại đại diện cho một khuôn mặt mới có chung các đặc điểm với hai khuôn mặt đã lưu. Như vậy, một sơ đồ xếp chồng là một sự trừu tượng đại diện cho các lớp của các đối tượng chứ không phải là các đối tượng riêng lẻ.</t>
+  </si>
+  <si>
+    <t>Với chính sách mở rộng này, chỉ số chứng khoán của Liên Hợp Quốc đã nhanh chóng tăng lên mức tích lũy  0,003% trong kỳ đầu tiên. Kết quả đạt được ở đây là phù hợp với thực tế tại Việt Nam, nơi mà việc mở rộng chính sách tiền tệ đã làm tăng cung tiền và nền kinh tế đang trong giai đoạn tăng trưởng, tạo cơ hội cho nhà đầu tư  tiếp cận nguồn vốn tín dụng giá rẻ. Cơ hội  mở rộng kinh doanh ngày càng nhiều. Do đó, cổ phiếu của công ty trở nên hấp dẫn hơn đối với các nhà đầu tư, dẫn đến giá cổ phiếu cao hơn, từ đó dẫn đến sự gia tăng của thị trường chứng khoán. 
+ CSGCK. Tuy nhiên, hình dạng hyperbol tăng và giảm của biểu đồ  cho thấy rằng các nhà đầu tư có thể không nghĩ rằng giá của chứng khoán sẽ tăng liên tục trong một thời gian dài. Trong trường hợp này lạm phát gây ra sự mất giá tiền tệ. Sau một thời gian, thị trường  điều chỉnh và biểu đồ đi xuống.</t>
+  </si>
+  <si>
+    <t>Các nghiên cứu này chủ yếu tập trung vào việc đo lường tác động của các yếu tố vĩ mô đến giá  cổ phiếu mà chưa xem xét tác động của các yếu tố cơ bản đối với công ty. Cũng theo quan sát của tác giả, thị trường vàng ở Việt Nam có quan hệ rất mật thiết với thị trường chứng khoán nên giá vàng là yếu tố có thể ảnh hưởng đến giá  cổ phiếu. Tuy nhiên, biến  này  không được sử dụng trong các nghiên cứu trước đây ở Việt Nam.</t>
+  </si>
+  <si>
+    <t>Các quá trình vật lý liên tục thay đổi trạng thái thường diễn ra trong khí quyển. Các điều kiện khí quyển  gần mặt đất và bên dưới (thường là trong môi trường  hàng không) được gọi là thời tiết. Các đặc điểm thời tiết như nhiệt độ, áp suất, độ ẩm, mây, lượng mưa và gió. 
+ Các hiện tượng như dông, bão, sương mù và gió Tây khô nóng được gọi là các yếu tố khí tượng.  Những thay đổi của thời tiết  gần bề mặt ảnh hưởng lớn đến nông nghiệp và các ngành công nghiệp khác của con người. Thời tiết  khí quyển trên cao  ảnh hưởng đến hoạt động bay. Cần lưu ý rằng các quá trình khí quyển ở các độ cao khác nhau có liên quan với nhau. Vì vậy, để nghiên cứu toàn diện thời tiết bề mặt, cần phải nghiên cứu cả  tầng khí quyển. Điều kiện khí quyển ở các lớp trên có xu hướng cao hơn về độ cao.</t>
+  </si>
+  <si>
+    <t>Sự hiện diện của khí quyển cũng rất quan trọng đối với các quá trình vật lý ở dưới đáy (trong đất) và các khối nước bên trên (xói mòn do gió,  dòng hải lưu, sóng  do gió gây ra, sự hình thành và tan chảy của tuyết, v.v.). hiện tượng) cũng như đối với sự sống trên Trái đất.</t>
+  </si>
+  <si>
+    <t>Những thay đổi cơ bản của thời tiết  liên quan đến sự  chuyển động của không khí trong hoàn lưu  khí quyển chung, khi các khối khí di chuyển từ vùng này sang vùng khác mang lại các điều kiện mới về nhiệt độ, độ ẩm,  mây che phủ và các yếu tố khác.</t>
+  </si>
+  <si>
+    <t>Được bảo vệ khỏi ảnh hưởng của dãy núi trung tâm phía tây bắc 
+ do có gió mùa đông bắc đi qua dãy Hoàng Liên Sơn nên  khí hậu đới B1 ấm hơn vùng đồng bằng bắc bộ ở phía nam, mùa mưa  sớm hơn, bão ít thiệt hại hơn, mùa hè nóng hơn nhiều.</t>
+  </si>
+  <si>
+    <t>Quy trình xác thực dữ liệu thủ công này  kiểm tra từng phần dữ liệu được liên kết với một mục, sửa mọi thông tin sai sót hoặc trùng lặp xuất hiện và xóa các mục không đáp ứng tiêu chí. của Simas.</t>
+  </si>
+  <si>
+    <t>Các chatbot ngày nay  sử dụng các kỹ thuật xử lý ngôn ngữ tự nhiên (NLP) tiên tiến, các kỹ thuật học sâu như học tăng cường sâu (DRL) và mạng nơ-ron sâu (DNN) [3]. Cộng đồng xử lý ngôn ngữ tự nhiên (NLP) đã đạt được những bước tiến lớn trong việc nhúng  ngữ cảnh và các mô hình ngôn ngữ hai chiều như BERT, RoBERTa và DitilBERT [4-8]. Đặc biệt, mô hình BERT (Devlin và cộng sự, 2019) đã trở thành nền tảng mới cho quá trình xử lý ngôn ngữ tự nhiên, bao gồm phân loại câu, trả lời câu hỏi và hơn thế nữa.</t>
+  </si>
+  <si>
+    <t>Một giải pháp được sử dụng là áp dụng  thuật toán phân loại cho chatbot để giảm  phân loại câu hỏi quá mức. Các câu hỏi  được phân loại theo các tiêu chí khác nhau để tạo ra một cấu trúc dễ quản lý hơn và tăng độ chính xác của câu trả lời mà chatbot cung cấp cho người dùng.</t>
+  </si>
+  <si>
+    <t>Trong thế giới sinh viên ngày nay,  đạo văn đã trở thành một hiện tượng đáng lo ngại, với việc sinh viên năm nhất, cuối cấp sao chép bài của nhau và “gạ” bài trên mạng mà không trích dẫn nguồn để nộp cho giáo viên hướng dẫn ngày càng tăng. Đối với họ, thực hiện phi vụ là một cuộc chạy trốn nhưng hậu quả thì khó lường.</t>
+  </si>
+  <si>
+    <t>Đạo văn là  sao chép, cắt, dán, gõ lại, viết lại hoặc sử dụng lại các ý tưởng hoặc kết quả mà không công nhận tác giả hoặc nguồn của thông tin. Đạo văn thường có hai dạng: sao chép nguyên văn và sao chép ý tưởng. Trong đạo văn, người sao chép  thu thập các đoạn văn bản từ nhiều nguồn khác nhau để tạo ra văn bản của riêng mình.</t>
+  </si>
+  <si>
+    <t>Tiền xử lý là một bước quan trọng đối với bất kỳ hệ thống tìm kiếm nào. Các tệp đầu vào có thể là .pdf, .doc hoặc .docx, đọc nội dung, xóa các ký tự đặc biệt (ký tự điều khiển, ngắt dòng, v.v.), thực hiện gạch nối câu, gạch nối từ và gắn nhãn.</t>
+  </si>
+  <si>
+    <t>Tận dụng đặc điểm của tiếng Việt là một ngôn ngữ đa âm, bài viết này trình bày phương pháp trích  từ khóa từ tài liệu tiếng Việt và sử dụng phương pháp này để trích xuất tài liệu  làm tiền đề cho việc giải quyết vấn đề phát hiện đạo văn đã giới thiệu thành công trong việc tra cứu.</t>
+  </si>
+  <si>
+    <t>Hiện tại  có một số giải pháp  phát hiện sao chép và một số công cụ phần mềm có thể được sử dụng để phát hiện liệu một tài liệu (được gọi là văn bản kiểm tra) đã được sao chép từ một tập hợp các tài liệu nguồn hay chưa. Các phương pháp này chủ yếu dựa vào tìm kiếm và đối sánh chuỗi, và chỉ  hiệu quả khi việc sao chép được thực hiện "bằng lời nói".</t>
+  </si>
+  <si>
+    <t>Với sự phát triển của Internet, thông tin được tạo ra liên tục hàng ngày, và lượng dữ liệu trên web là vô cùng lớn nên thường xuyên xảy ra vấn đề trùng lặp thông tin. Giải pháp cho vấn đề này  là tự động tóm tắt văn bản. Tóm tắt  giúp người dùng tiết kiệm thời gian đọc, cải thiện tìm kiếm và tăng hiệu quả lập chỉ mục của công cụ tìm kiếm.</t>
+  </si>
+  <si>
+    <t>Các công cụ khai thác dữ liệu có thể phát hiện ra các xu hướng trong tương lai. Kiến thức mà khai thác dữ liệu mang lại cho  doanh nghiệp của bạn có thể giúp bạn đưa ra  quyết định kịp thời và trả lời các câu hỏi  kinh doanh chưa biết trước đây.</t>
+  </si>
+  <si>
+    <t>Hầu hết các tổ chức chính phủ, công nghiệp, thương mại và  nghiên cứu  lưu trữ thông tin của họ dưới dạng điện tử theo kiểu cơ sở dữ liệu văn bản. Số lượng tài liệu điện tử này đang tăng lên nhanh chóng, khiến người ta khó tiếp thu những  nội dung trọng tâm. Các kỹ thuật truy xuất thông tin truyền thống đang trở nên không cân xứng với lượng dữ liệu văn bản ngày càng tăng. Người dùng không hiểu nội dung của tài liệu nên khó thực hiện các truy vấn hiệu quả để phân tích dữ liệu và trích xuất thông tin hữu ích. Người dùng cần các công cụ để so sánh các tài liệu khác nhau, xếp hạng các tài liệu về mức độ quan trọng và mức độ liên quan, đồng thời tìm ra các mẫu và  xu hướng trên các tài liệu. Vì vậy, việc tính toán độ giống nhau giữa các văn bản, độ giống nhau giữa các văn bản, tóm tắt văn bản,… đang được phổ biến và trở thành một nội dung  thiết yếu trong khai thác văn bản.</t>
   </si>
 </sst>
 </file>
@@ -680,21 +793,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9E00F2-0038-415A-AC77-D737CE8651F6}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="13.9" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.46484375" style="1"/>
-    <col min="2" max="2" width="61.265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.9296875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.46484375" style="1"/>
+    <col min="2" max="2" width="62.46484375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.9296875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.46484375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,339 +816,432 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="263.64999999999998" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="263.64999999999998" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="346.9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="346.9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="208.15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="208.15" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="111" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="111" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="97.15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="97.15" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="111" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="124.9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="69.400000000000006" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="69.400000000000006" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="97.15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="97.15" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="69.400000000000006" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="69.400000000000006" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="83.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="83.25" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="41.65" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="374.65" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="374.65" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="166.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="166.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="83.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="83.25" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="194.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="194.25" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="69.400000000000006" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="69.400000000000006" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="41.65" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="41.65" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="97.15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="97.15" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="69.400000000000006" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" ht="69.400000000000006" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="69.400000000000006" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" ht="69.400000000000006" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="69.400000000000006" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" ht="69.400000000000006" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="69.400000000000006" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" ht="69.400000000000006" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="166.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" ht="166.5" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>